<commit_message>
Make columns dynamics from keys of a obj from data
</commit_message>
<xml_diff>
--- a/reports/Academics_18.05.2021.xlsx
+++ b/reports/Academics_18.05.2021.xlsx
@@ -11,51 +11,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
-  <si>
-    <t>CR No</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Assignment</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+  <si>
+    <t>CRNO</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>SEX</t>
+  </si>
+  <si>
+    <t>TOPICS</t>
+  </si>
+  <si>
+    <t>WORK</t>
+  </si>
+  <si>
+    <t>Gurkeerat</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Alphabets</t>
+  </si>
+  <si>
+    <t>Gurjashan</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Tables 2 - 10</t>
+  </si>
+  <si>
+    <t>Rayna</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>Gurkeerat</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Alphabets</t>
-  </si>
-  <si>
-    <t>Gurjashan</t>
-  </si>
-  <si>
-    <t>Maths</t>
-  </si>
-  <si>
-    <t>Tables 2 - 10</t>
-  </si>
-  <si>
-    <t>Rayna</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
   <si>
     <t>Reasoning</t>
@@ -546,10 +549,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -557,7 +560,7 @@
         <v>226334</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -566,10 +569,10 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -577,7 +580,7 @@
         <v>284692</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
         <v>10</v>
@@ -589,15 +592,15 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>

</xml_diff>